<commit_message>
SCE reduced results till 2022 m10
</commit_message>
<xml_diff>
--- a/workingfolder/tables/reduced_form_results/RVEffResult_new.xlsx
+++ b/workingfolder/tables/reduced_form_results/RVEffResult_new.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10911"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tao/Dropbox/InfVar/workingfolder/tables/reduced_form_results/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Myworld/Dropbox/InfVar/workingfolder/tables/reduced_form_results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A43CDD72-AEC0-7844-A6E5-86DF345E83A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF7169E4-B241-8646-81A2-7A3548E00A57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="23500" windowHeight="15620" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="23500" windowHeight="13820" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Export Summary" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="354" uniqueCount="154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="354" uniqueCount="153">
   <si>
     <t>This document was exported from Numbers.  Each table was converted to an Excel worksheet. All other objects on each Numbers sheet were placed on separate worksheets. Please be aware that formula calculations may differ in Excel.</t>
   </si>
@@ -244,9 +244,6 @@
     <t>0.439</t>
   </si>
   <si>
-    <t>0.448</t>
-  </si>
-  <si>
     <t>0.393</t>
   </si>
   <si>
@@ -292,18 +289,6 @@
     <t>(0.003)</t>
   </si>
   <si>
-    <t>74</t>
-  </si>
-  <si>
-    <t>50</t>
-  </si>
-  <si>
-    <t>49</t>
-  </si>
-  <si>
-    <t>48</t>
-  </si>
-  <si>
     <t>0.000</t>
   </si>
   <si>
@@ -325,18 +310,9 @@
     <t>L26.InfExp_Mean_rv</t>
   </si>
   <si>
-    <t>-0.106</t>
-  </si>
-  <si>
     <t>(0.054)</t>
   </si>
   <si>
-    <t>(0.080)</t>
-  </si>
-  <si>
-    <t>(0.074)</t>
-  </si>
-  <si>
     <t>24m before</t>
   </si>
   <si>
@@ -394,118 +370,139 @@
     <t>5 q before</t>
   </si>
   <si>
-    <t>0.233*</t>
-  </si>
-  <si>
-    <t>(0.100)</t>
-  </si>
-  <si>
-    <t>0.225*</t>
-  </si>
-  <si>
-    <t>(0.103)</t>
-  </si>
-  <si>
-    <t>0.254*</t>
-  </si>
-  <si>
-    <t>(0.098)</t>
-  </si>
-  <si>
     <t>L12.InfExp_FE</t>
   </si>
   <si>
-    <t>-0.330***</t>
-  </si>
-  <si>
-    <t>-0.327***</t>
-  </si>
-  <si>
-    <t>-0.331***</t>
-  </si>
-  <si>
-    <t>0.504***</t>
-  </si>
-  <si>
-    <t>0.510***</t>
-  </si>
-  <si>
-    <t>0.530***</t>
-  </si>
-  <si>
-    <t>0.595</t>
-  </si>
-  <si>
-    <t>0.600</t>
-  </si>
-  <si>
-    <t>0.616</t>
-  </si>
-  <si>
-    <t>-0.679**</t>
-  </si>
-  <si>
-    <t>(0.202)</t>
-  </si>
-  <si>
-    <t>-0.740**</t>
-  </si>
-  <si>
-    <t>(0.216)</t>
-  </si>
-  <si>
-    <t>-0.874***</t>
-  </si>
-  <si>
-    <t>(0.201)</t>
-  </si>
-  <si>
-    <t>0.568***</t>
-  </si>
-  <si>
-    <t>0.600***</t>
-  </si>
-  <si>
-    <t>(0.101)</t>
-  </si>
-  <si>
-    <t>(0.092)</t>
-  </si>
-  <si>
-    <t>(0.091)</t>
-  </si>
-  <si>
     <t>L12.InfExp_FE2</t>
   </si>
   <si>
-    <t>0.114</t>
-  </si>
-  <si>
-    <t>-1.121***</t>
-  </si>
-  <si>
-    <t>-1.237***</t>
-  </si>
-  <si>
-    <t>-1.366***</t>
-  </si>
-  <si>
-    <t>(0.180)</t>
-  </si>
-  <si>
-    <t>(0.247)</t>
-  </si>
-  <si>
-    <t>(0.204)</t>
-  </si>
-  <si>
-    <t>(0.237)</t>
-  </si>
-  <si>
-    <t>0.372</t>
-  </si>
-  <si>
-    <t>0.402</t>
+    <t>-0.666***</t>
+  </si>
+  <si>
+    <t>(0.151)</t>
+  </si>
+  <si>
+    <t>-0.501*</t>
+  </si>
+  <si>
+    <t>(0.208)</t>
+  </si>
+  <si>
+    <t>-0.376</t>
+  </si>
+  <si>
+    <t>(0.219)</t>
+  </si>
+  <si>
+    <t>0.357***</t>
+  </si>
+  <si>
+    <t>0.328***</t>
+  </si>
+  <si>
+    <t>0.306***</t>
+  </si>
+  <si>
+    <t>(0.039)</t>
+  </si>
+  <si>
+    <t>0.778***</t>
+  </si>
+  <si>
+    <t>-0.623*</t>
+  </si>
+  <si>
+    <t>-0.426</t>
+  </si>
+  <si>
+    <t>-0.275</t>
+  </si>
+  <si>
+    <t>(0.225)</t>
+  </si>
+  <si>
+    <t>(0.272)</t>
+  </si>
+  <si>
+    <t>(0.337)</t>
+  </si>
+  <si>
+    <t>(0.345)</t>
+  </si>
+  <si>
+    <t>0.527</t>
+  </si>
+  <si>
+    <t>0.498</t>
+  </si>
+  <si>
+    <t>0.478</t>
+  </si>
+  <si>
+    <t>88</t>
+  </si>
+  <si>
+    <t>64</t>
+  </si>
+  <si>
+    <t>63</t>
+  </si>
+  <si>
+    <t>62</t>
+  </si>
+  <si>
+    <t>0.328**</t>
+  </si>
+  <si>
+    <t>(0.104)</t>
+  </si>
+  <si>
+    <t>0.334**</t>
+  </si>
+  <si>
+    <t>(0.106)</t>
+  </si>
+  <si>
+    <t>0.382***</t>
+  </si>
+  <si>
+    <t>(0.099)</t>
+  </si>
+  <si>
+    <t>-0.462***</t>
+  </si>
+  <si>
+    <t>-0.460***</t>
+  </si>
+  <si>
+    <t>-0.459***</t>
+  </si>
+  <si>
+    <t>(0.016)</t>
+  </si>
+  <si>
+    <t>0.365**</t>
+  </si>
+  <si>
+    <t>0.781***</t>
+  </si>
+  <si>
+    <t>0.790***</t>
+  </si>
+  <si>
+    <t>0.807***</t>
+  </si>
+  <si>
+    <t>(0.111)</t>
+  </si>
+  <si>
+    <t>0.924</t>
+  </si>
+  <si>
+    <t>0.926</t>
+  </si>
+  <si>
+    <t>0.931</t>
   </si>
 </sst>
 </file>
@@ -929,6 +926,16 @@
     <xf numFmtId="0" fontId="3" fillId="8" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="3" fillId="8" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="8" borderId="16" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="15" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="8" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="8" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="3" fillId="8" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -957,16 +964,6 @@
     <xf numFmtId="49" fontId="0" fillId="9" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="15" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="8" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="8" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="3" fillId="8" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2159,11 +2156,11 @@
     </row>
     <row r="3" spans="1:5" ht="50" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="8"/>
-      <c r="B3" s="73" t="s">
+      <c r="B3" s="81" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="74"/>
-      <c r="D3" s="74"/>
+      <c r="C3" s="82"/>
+      <c r="D3" s="82"/>
       <c r="E3" s="10"/>
     </row>
     <row r="4" spans="1:5" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -2286,8 +2283,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:O77"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A8" zoomScale="83" workbookViewId="0">
-      <selection activeCell="R42" sqref="R42"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A3" zoomScale="83" workbookViewId="0">
+      <selection activeCell="P17" sqref="P17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2303,44 +2300,44 @@
     <row r="1" spans="1:15" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="19"/>
       <c r="B1" s="20"/>
-      <c r="C1" s="75" t="s">
+      <c r="C1" s="83" t="s">
         <v>8</v>
       </c>
-      <c r="D1" s="76"/>
-      <c r="E1" s="76"/>
-      <c r="F1" s="76"/>
-      <c r="G1" s="75" t="s">
+      <c r="D1" s="84"/>
+      <c r="E1" s="84"/>
+      <c r="F1" s="84"/>
+      <c r="G1" s="83" t="s">
         <v>9</v>
       </c>
-      <c r="H1" s="76"/>
-      <c r="I1" s="76"/>
-      <c r="J1" s="76"/>
+      <c r="H1" s="84"/>
+      <c r="I1" s="84"/>
+      <c r="J1" s="84"/>
       <c r="K1" s="21"/>
-      <c r="L1" s="75" t="s">
+      <c r="L1" s="83" t="s">
         <v>10</v>
       </c>
-      <c r="M1" s="76"/>
-      <c r="N1" s="76"/>
-      <c r="O1" s="77"/>
+      <c r="M1" s="84"/>
+      <c r="N1" s="84"/>
+      <c r="O1" s="85"/>
     </row>
     <row r="2" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="22"/>
-      <c r="B2" s="81" t="s">
+      <c r="B2" s="89" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="81"/>
-      <c r="D2" s="81"/>
-      <c r="E2" s="81"/>
-      <c r="F2" s="81"/>
-      <c r="G2" s="81"/>
-      <c r="H2" s="81"/>
-      <c r="I2" s="81"/>
-      <c r="J2" s="81"/>
-      <c r="K2" s="81"/>
-      <c r="L2" s="81"/>
-      <c r="M2" s="81"/>
-      <c r="N2" s="81"/>
-      <c r="O2" s="82"/>
+      <c r="C2" s="89"/>
+      <c r="D2" s="89"/>
+      <c r="E2" s="89"/>
+      <c r="F2" s="89"/>
+      <c r="G2" s="89"/>
+      <c r="H2" s="89"/>
+      <c r="I2" s="89"/>
+      <c r="J2" s="89"/>
+      <c r="K2" s="89"/>
+      <c r="L2" s="89"/>
+      <c r="M2" s="89"/>
+      <c r="N2" s="89"/>
+      <c r="O2" s="90"/>
     </row>
     <row r="3" spans="1:15" ht="48" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="22"/>
@@ -2349,38 +2346,38 @@
         <v>12</v>
       </c>
       <c r="D3" s="40" t="s">
-        <v>114</v>
+        <v>106</v>
       </c>
       <c r="E3" s="40" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F3" s="40" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
       <c r="G3" s="23" t="s">
         <v>12</v>
       </c>
       <c r="H3" s="23" t="s">
+        <v>70</v>
+      </c>
+      <c r="I3" s="23" t="s">
         <v>71</v>
       </c>
-      <c r="I3" s="23" t="s">
+      <c r="J3" s="23" t="s">
         <v>72</v>
-      </c>
-      <c r="J3" s="23" t="s">
-        <v>73</v>
       </c>
       <c r="K3" s="24"/>
       <c r="L3" s="23" t="s">
         <v>12</v>
       </c>
       <c r="M3" s="23" t="s">
-        <v>97</v>
+        <v>89</v>
       </c>
       <c r="N3" s="23" t="s">
-        <v>98</v>
+        <v>90</v>
       </c>
       <c r="O3" s="25" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
     </row>
     <row r="4" spans="1:15" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -2413,13 +2410,13 @@
         <v>41</v>
       </c>
       <c r="K4" s="49" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="L4" s="54" t="s">
         <v>41</v>
       </c>
       <c r="M4" s="42" t="s">
-        <v>116</v>
+        <v>135</v>
       </c>
       <c r="N4" s="42" t="s">
         <v>41</v>
@@ -2464,7 +2461,7 @@
         <v>41</v>
       </c>
       <c r="M5" s="43" t="s">
-        <v>117</v>
+        <v>136</v>
       </c>
       <c r="N5" s="43" t="s">
         <v>41</v>
@@ -2516,7 +2513,7 @@
       </c>
       <c r="J7" s="43"/>
       <c r="K7" s="44" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="L7" s="45" t="s">
         <v>41</v>
@@ -2525,7 +2522,7 @@
         <v>41</v>
       </c>
       <c r="N7" s="43" t="s">
-        <v>118</v>
+        <v>137</v>
       </c>
       <c r="O7" s="43" t="s">
         <v>41</v>
@@ -2566,7 +2563,7 @@
         <v>41</v>
       </c>
       <c r="N8" s="43" t="s">
-        <v>119</v>
+        <v>138</v>
       </c>
       <c r="O8" s="43" t="s">
         <v>41</v>
@@ -2604,7 +2601,7 @@
         <v>41</v>
       </c>
       <c r="F10" s="43" t="s">
-        <v>100</v>
+        <v>92</v>
       </c>
       <c r="G10" s="44" t="s">
         <v>41</v>
@@ -2619,7 +2616,7 @@
         <v>47</v>
       </c>
       <c r="K10" s="44" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="L10" s="45" t="s">
         <v>41</v>
@@ -2631,7 +2628,7 @@
         <v>41</v>
       </c>
       <c r="O10" s="43" t="s">
-        <v>120</v>
+        <v>139</v>
       </c>
     </row>
     <row r="11" spans="1:15" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -2649,7 +2646,7 @@
         <v>41</v>
       </c>
       <c r="F11" s="43" t="s">
-        <v>101</v>
+        <v>93</v>
       </c>
       <c r="G11" s="44" t="s">
         <v>41</v>
@@ -2661,7 +2658,7 @@
         <v>41</v>
       </c>
       <c r="J11" s="43" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="K11" s="44" t="s">
         <v>41</v>
@@ -2676,7 +2673,7 @@
         <v>41</v>
       </c>
       <c r="O11" s="43" t="s">
-        <v>121</v>
+        <v>140</v>
       </c>
     </row>
     <row r="12" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -2708,19 +2705,19 @@
       <c r="I13" s="43"/>
       <c r="J13" s="43"/>
       <c r="K13" s="44" t="s">
-        <v>122</v>
+        <v>108</v>
       </c>
       <c r="L13" s="45" t="s">
         <v>41</v>
       </c>
       <c r="M13" s="45" t="s">
-        <v>123</v>
+        <v>141</v>
       </c>
       <c r="N13" s="45" t="s">
-        <v>124</v>
+        <v>142</v>
       </c>
       <c r="O13" s="43" t="s">
-        <v>125</v>
+        <v>143</v>
       </c>
     </row>
     <row r="14" spans="1:15" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -2741,13 +2738,13 @@
         <v>41</v>
       </c>
       <c r="M14" s="45" t="s">
-        <v>101</v>
+        <v>144</v>
       </c>
       <c r="N14" s="45" t="s">
-        <v>48</v>
+        <v>144</v>
       </c>
       <c r="O14" s="43" t="s">
-        <v>48</v>
+        <v>144</v>
       </c>
     </row>
     <row r="15" spans="1:15" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -2794,22 +2791,22 @@
         <v>56</v>
       </c>
       <c r="J16" s="43" t="s">
-        <v>104</v>
+        <v>96</v>
       </c>
       <c r="K16" s="51" t="s">
         <v>60</v>
       </c>
       <c r="L16" s="43" t="s">
-        <v>93</v>
+        <v>145</v>
       </c>
       <c r="M16" s="43" t="s">
-        <v>126</v>
+        <v>146</v>
       </c>
       <c r="N16" s="43" t="s">
-        <v>127</v>
+        <v>147</v>
       </c>
       <c r="O16" s="43" t="s">
-        <v>128</v>
+        <v>148</v>
       </c>
     </row>
     <row r="17" spans="1:15" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -2843,16 +2840,16 @@
       </c>
       <c r="K17" s="50"/>
       <c r="L17" s="43" t="s">
-        <v>94</v>
+        <v>149</v>
       </c>
       <c r="M17" s="43" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="N17" s="43" t="s">
-        <v>95</v>
+        <v>48</v>
       </c>
       <c r="O17" s="43" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="18" spans="1:15" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -2870,34 +2867,34 @@
         <v>65</v>
       </c>
       <c r="F18" s="43" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="G18" s="43" t="s">
+        <v>66</v>
+      </c>
+      <c r="H18" s="43" t="s">
         <v>67</v>
       </c>
-      <c r="H18" s="43" t="s">
+      <c r="I18" s="43" t="s">
         <v>68</v>
       </c>
-      <c r="I18" s="43" t="s">
-        <v>69</v>
-      </c>
       <c r="J18" s="43" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="K18" s="51" t="s">
         <v>23</v>
       </c>
       <c r="L18" s="43" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="M18" s="43" t="s">
-        <v>129</v>
+        <v>150</v>
       </c>
       <c r="N18" s="43" t="s">
-        <v>130</v>
+        <v>151</v>
       </c>
       <c r="O18" s="43" t="s">
-        <v>131</v>
+        <v>152</v>
       </c>
     </row>
     <row r="19" spans="1:15" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -2915,7 +2912,7 @@
         <v>1290</v>
       </c>
       <c r="F19" s="52" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
       <c r="G19" s="52">
         <v>1362</v>
@@ -2927,28 +2924,28 @@
         <v>1033</v>
       </c>
       <c r="J19" s="52" t="s">
-        <v>105</v>
+        <v>97</v>
       </c>
       <c r="K19" s="51" t="s">
         <v>22</v>
       </c>
       <c r="L19" s="43" t="s">
-        <v>82</v>
+        <v>131</v>
       </c>
       <c r="M19" s="43" t="s">
-        <v>83</v>
+        <v>132</v>
       </c>
       <c r="N19" s="43" t="s">
-        <v>84</v>
+        <v>133</v>
       </c>
       <c r="O19" s="43" t="s">
-        <v>85</v>
+        <v>134</v>
       </c>
     </row>
     <row r="20" spans="1:15" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="19"/>
       <c r="B20" s="53" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C20" s="53" t="s">
         <v>61</v>
@@ -2975,7 +2972,7 @@
         <v>61</v>
       </c>
       <c r="K20" s="62" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="L20" s="62" t="s">
         <v>62</v>
@@ -3009,22 +3006,22 @@
     </row>
     <row r="22" spans="1:15" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="19"/>
-      <c r="B22" s="78" t="s">
+      <c r="B22" s="86" t="s">
         <v>24</v>
       </c>
-      <c r="C22" s="79"/>
-      <c r="D22" s="79"/>
-      <c r="E22" s="79"/>
-      <c r="F22" s="79"/>
-      <c r="G22" s="79"/>
-      <c r="H22" s="79"/>
-      <c r="I22" s="79"/>
-      <c r="J22" s="79"/>
-      <c r="K22" s="80"/>
-      <c r="L22" s="79"/>
-      <c r="M22" s="79"/>
-      <c r="N22" s="79"/>
-      <c r="O22" s="79"/>
+      <c r="C22" s="87"/>
+      <c r="D22" s="87"/>
+      <c r="E22" s="87"/>
+      <c r="F22" s="87"/>
+      <c r="G22" s="87"/>
+      <c r="H22" s="87"/>
+      <c r="I22" s="87"/>
+      <c r="J22" s="87"/>
+      <c r="K22" s="88"/>
+      <c r="L22" s="87"/>
+      <c r="M22" s="87"/>
+      <c r="N22" s="87"/>
+      <c r="O22" s="87"/>
     </row>
     <row r="23" spans="1:15" ht="32" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="19"/>
@@ -3033,38 +3030,38 @@
         <v>12</v>
       </c>
       <c r="D23" s="40" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E23" s="40" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F23" s="40" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
       <c r="G23" s="23" t="s">
         <v>12</v>
       </c>
       <c r="H23" s="40" t="s">
+        <v>71</v>
+      </c>
+      <c r="I23" s="23" t="s">
+        <v>71</v>
+      </c>
+      <c r="J23" s="23" t="s">
         <v>72</v>
-      </c>
-      <c r="I23" s="23" t="s">
-        <v>72</v>
-      </c>
-      <c r="J23" s="23" t="s">
-        <v>73</v>
       </c>
       <c r="K23" s="34"/>
       <c r="L23" s="23" t="s">
         <v>12</v>
       </c>
       <c r="M23" s="40" t="s">
-        <v>97</v>
+        <v>89</v>
       </c>
       <c r="N23" s="40" t="s">
-        <v>98</v>
+        <v>90</v>
       </c>
       <c r="O23" s="63" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
     </row>
     <row r="24" spans="1:15" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -3075,7 +3072,7 @@
       </c>
       <c r="C24" s="66"/>
       <c r="D24" s="42" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E24" s="42" t="s">
         <v>16</v>
@@ -3083,20 +3080,20 @@
       <c r="F24" s="42"/>
       <c r="G24" s="66"/>
       <c r="H24" s="42" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="I24" s="42" t="s">
         <v>25</v>
       </c>
       <c r="J24" s="42"/>
       <c r="K24" s="44" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="L24" s="54" t="s">
         <v>41</v>
       </c>
       <c r="M24" s="42" t="s">
-        <v>132</v>
+        <v>110</v>
       </c>
       <c r="N24" s="42" t="s">
         <v>41</v>
@@ -3113,7 +3110,7 @@
       </c>
       <c r="C25" s="66"/>
       <c r="D25" s="43" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E25" s="43" t="s">
         <v>18</v>
@@ -3134,7 +3131,7 @@
         <v>41</v>
       </c>
       <c r="M25" s="43" t="s">
-        <v>133</v>
+        <v>111</v>
       </c>
       <c r="N25" s="43" t="s">
         <v>41</v>
@@ -3174,7 +3171,7 @@
         <v>41</v>
       </c>
       <c r="F27" s="43" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
       <c r="G27" s="66"/>
       <c r="H27" s="43" t="s">
@@ -3184,10 +3181,10 @@
         <v>41</v>
       </c>
       <c r="J27" s="43" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="K27" s="44" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="L27" s="45" t="s">
         <v>41</v>
@@ -3196,7 +3193,7 @@
         <v>41</v>
       </c>
       <c r="N27" s="43" t="s">
-        <v>134</v>
+        <v>112</v>
       </c>
       <c r="O27" s="43" t="s">
         <v>41</v>
@@ -3213,7 +3210,7 @@
         <v>41</v>
       </c>
       <c r="F28" s="43" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
       <c r="G28" s="66"/>
       <c r="H28" s="43" t="s">
@@ -3223,7 +3220,7 @@
         <v>41</v>
       </c>
       <c r="J28" s="43" t="s">
-        <v>110</v>
+        <v>102</v>
       </c>
       <c r="K28" s="44" t="s">
         <v>41</v>
@@ -3235,7 +3232,7 @@
         <v>41</v>
       </c>
       <c r="N28" s="43" t="s">
-        <v>135</v>
+        <v>113</v>
       </c>
       <c r="O28" s="43" t="s">
         <v>41</v>
@@ -3281,17 +3278,17 @@
     </row>
     <row r="30" spans="1:15" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="22"/>
-      <c r="B30" s="84"/>
-      <c r="C30" s="84"/>
-      <c r="D30" s="84"/>
-      <c r="E30" s="84"/>
-      <c r="F30" s="84"/>
-      <c r="G30" s="84"/>
-      <c r="H30" s="84"/>
-      <c r="I30" s="84"/>
-      <c r="J30" s="84"/>
+      <c r="B30" s="74"/>
+      <c r="C30" s="74"/>
+      <c r="D30" s="74"/>
+      <c r="E30" s="74"/>
+      <c r="F30" s="74"/>
+      <c r="G30" s="74"/>
+      <c r="H30" s="74"/>
+      <c r="I30" s="74"/>
+      <c r="J30" s="74"/>
       <c r="K30" s="72" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="L30" s="45" t="s">
         <v>41</v>
@@ -3303,20 +3300,20 @@
         <v>41</v>
       </c>
       <c r="O30" s="43" t="s">
-        <v>136</v>
+        <v>114</v>
       </c>
     </row>
     <row r="31" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="22"/>
-      <c r="B31" s="84"/>
-      <c r="C31" s="84"/>
-      <c r="D31" s="84"/>
-      <c r="E31" s="84"/>
-      <c r="F31" s="84"/>
-      <c r="G31" s="84"/>
-      <c r="H31" s="84"/>
-      <c r="I31" s="84"/>
-      <c r="J31" s="84"/>
+      <c r="B31" s="74"/>
+      <c r="C31" s="74"/>
+      <c r="D31" s="74"/>
+      <c r="E31" s="74"/>
+      <c r="F31" s="74"/>
+      <c r="G31" s="74"/>
+      <c r="H31" s="74"/>
+      <c r="I31" s="74"/>
+      <c r="J31" s="74"/>
       <c r="K31" s="72" t="s">
         <v>41</v>
       </c>
@@ -3330,21 +3327,21 @@
         <v>41</v>
       </c>
       <c r="O31" s="43" t="s">
-        <v>137</v>
+        <v>115</v>
       </c>
     </row>
     <row r="32" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="22"/>
-      <c r="B32" s="85"/>
-      <c r="C32" s="85"/>
-      <c r="D32" s="85"/>
-      <c r="E32" s="85"/>
-      <c r="F32" s="85"/>
-      <c r="G32" s="85"/>
-      <c r="H32" s="85"/>
-      <c r="I32" s="85"/>
-      <c r="J32" s="85"/>
-      <c r="K32" s="86"/>
+      <c r="B32" s="75"/>
+      <c r="C32" s="75"/>
+      <c r="D32" s="75"/>
+      <c r="E32" s="75"/>
+      <c r="F32" s="75"/>
+      <c r="G32" s="75"/>
+      <c r="H32" s="75"/>
+      <c r="I32" s="75"/>
+      <c r="J32" s="75"/>
+      <c r="K32" s="76"/>
       <c r="L32" s="70"/>
       <c r="M32" s="70"/>
       <c r="N32" s="70"/>
@@ -3352,29 +3349,29 @@
     </row>
     <row r="33" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="22"/>
-      <c r="B33" s="85"/>
-      <c r="C33" s="85"/>
-      <c r="D33" s="85"/>
-      <c r="E33" s="85"/>
-      <c r="F33" s="85"/>
-      <c r="G33" s="85"/>
-      <c r="H33" s="85"/>
-      <c r="I33" s="85"/>
-      <c r="J33" s="85"/>
-      <c r="K33" s="86" t="s">
-        <v>143</v>
+      <c r="B33" s="75"/>
+      <c r="C33" s="75"/>
+      <c r="D33" s="75"/>
+      <c r="E33" s="75"/>
+      <c r="F33" s="75"/>
+      <c r="G33" s="75"/>
+      <c r="H33" s="75"/>
+      <c r="I33" s="75"/>
+      <c r="J33" s="75"/>
+      <c r="K33" s="76" t="s">
+        <v>109</v>
       </c>
       <c r="L33" s="70" t="s">
         <v>41</v>
       </c>
       <c r="M33" s="70" t="s">
-        <v>127</v>
+        <v>116</v>
       </c>
       <c r="N33" s="70" t="s">
-        <v>138</v>
+        <v>117</v>
       </c>
       <c r="O33" s="71" t="s">
-        <v>139</v>
+        <v>118</v>
       </c>
     </row>
     <row r="34" spans="1:15" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -3393,13 +3390,13 @@
         <v>41</v>
       </c>
       <c r="M34" s="70" t="s">
-        <v>140</v>
+        <v>119</v>
       </c>
       <c r="N34" s="70" t="s">
-        <v>141</v>
+        <v>18</v>
       </c>
       <c r="O34" s="71" t="s">
-        <v>142</v>
+        <v>75</v>
       </c>
     </row>
     <row r="35" spans="1:15" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -3412,12 +3409,12 @@
       <c r="G35" s="54"/>
       <c r="H35" s="54"/>
       <c r="I35" s="54"/>
-      <c r="J35" s="87"/>
-      <c r="K35" s="88"/>
-      <c r="L35" s="89"/>
-      <c r="M35" s="89"/>
-      <c r="N35" s="89"/>
-      <c r="O35" s="90"/>
+      <c r="J35" s="77"/>
+      <c r="K35" s="78"/>
+      <c r="L35" s="79"/>
+      <c r="M35" s="79"/>
+      <c r="N35" s="79"/>
+      <c r="O35" s="80"/>
     </row>
     <row r="36" spans="1:15" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="19"/>
@@ -3425,43 +3422,43 @@
         <v>60</v>
       </c>
       <c r="C36" s="43" t="s">
+        <v>76</v>
+      </c>
+      <c r="D36" s="43" t="s">
         <v>77</v>
-      </c>
-      <c r="D36" s="43" t="s">
-        <v>78</v>
       </c>
       <c r="E36" s="43" t="s">
         <v>26</v>
       </c>
       <c r="F36" s="43" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G36" s="43" t="s">
         <v>39</v>
       </c>
       <c r="H36" s="43" t="s">
+        <v>78</v>
+      </c>
+      <c r="I36" s="43" t="s">
         <v>79</v>
       </c>
-      <c r="I36" s="43" t="s">
-        <v>80</v>
-      </c>
       <c r="J36" s="55" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="K36" s="57" t="s">
         <v>60</v>
       </c>
       <c r="L36" s="58" t="s">
-        <v>144</v>
+        <v>120</v>
       </c>
       <c r="M36" s="58" t="s">
-        <v>145</v>
+        <v>121</v>
       </c>
       <c r="N36" s="58" t="s">
-        <v>146</v>
+        <v>122</v>
       </c>
       <c r="O36" s="58" t="s">
-        <v>147</v>
+        <v>123</v>
       </c>
     </row>
     <row r="37" spans="1:15" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -3489,23 +3486,23 @@
         <v>28</v>
       </c>
       <c r="I37" s="43" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="J37" s="55" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="K37" s="58"/>
       <c r="L37" s="58" t="s">
-        <v>148</v>
+        <v>124</v>
       </c>
       <c r="M37" s="58" t="s">
-        <v>149</v>
+        <v>125</v>
       </c>
       <c r="N37" s="58" t="s">
-        <v>150</v>
+        <v>126</v>
       </c>
       <c r="O37" s="58" t="s">
-        <v>151</v>
+        <v>127</v>
       </c>
     </row>
     <row r="38" spans="1:15" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -3557,7 +3554,7 @@
         <v>0.248</v>
       </c>
       <c r="F40" s="47" t="s">
-        <v>108</v>
+        <v>100</v>
       </c>
       <c r="G40" s="47">
         <v>5.3999999999999999E-2</v>
@@ -3569,22 +3566,22 @@
         <v>0.215</v>
       </c>
       <c r="J40" s="47" t="s">
-        <v>112</v>
+        <v>104</v>
       </c>
       <c r="K40" s="60" t="s">
         <v>23</v>
       </c>
       <c r="L40" s="61" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="M40" s="61" t="s">
-        <v>152</v>
+        <v>128</v>
       </c>
       <c r="N40" s="61" t="s">
-        <v>153</v>
+        <v>129</v>
       </c>
       <c r="O40" s="61" t="s">
-        <v>66</v>
+        <v>130</v>
       </c>
     </row>
     <row r="41" spans="1:15" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -3601,7 +3598,7 @@
       <c r="E41" s="47">
         <v>1157</v>
       </c>
-      <c r="F41" s="83">
+      <c r="F41" s="73">
         <v>1021</v>
       </c>
       <c r="G41" s="47">
@@ -3620,22 +3617,22 @@
         <v>22</v>
       </c>
       <c r="L41" s="61" t="s">
-        <v>82</v>
+        <v>131</v>
       </c>
       <c r="M41" s="61" t="s">
-        <v>83</v>
+        <v>132</v>
       </c>
       <c r="N41" s="61" t="s">
-        <v>84</v>
+        <v>133</v>
       </c>
       <c r="O41" s="61" t="s">
-        <v>85</v>
+        <v>134</v>
       </c>
     </row>
     <row r="42" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="19"/>
       <c r="B42" s="48" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C42" s="47" t="s">
         <v>61</v>
@@ -3662,7 +3659,7 @@
         <v>61</v>
       </c>
       <c r="K42" s="67" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="L42" s="68" t="s">
         <v>62</v>
@@ -4306,25 +4303,25 @@
     <row r="1" spans="1:15" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="19"/>
       <c r="B1" s="33"/>
-      <c r="C1" s="75" t="s">
+      <c r="C1" s="83" t="s">
         <v>8</v>
       </c>
-      <c r="D1" s="76"/>
-      <c r="E1" s="76"/>
-      <c r="F1" s="76"/>
-      <c r="G1" s="75" t="s">
+      <c r="D1" s="84"/>
+      <c r="E1" s="84"/>
+      <c r="F1" s="84"/>
+      <c r="G1" s="83" t="s">
         <v>9</v>
       </c>
-      <c r="H1" s="76"/>
-      <c r="I1" s="76"/>
-      <c r="J1" s="76"/>
+      <c r="H1" s="84"/>
+      <c r="I1" s="84"/>
+      <c r="J1" s="84"/>
       <c r="K1" s="21"/>
-      <c r="L1" s="75" t="s">
+      <c r="L1" s="83" t="s">
         <v>10</v>
       </c>
-      <c r="M1" s="76"/>
-      <c r="N1" s="76"/>
-      <c r="O1" s="77"/>
+      <c r="M1" s="84"/>
+      <c r="N1" s="84"/>
+      <c r="O1" s="85"/>
     </row>
     <row r="2" spans="1:15" ht="57" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="19"/>

</xml_diff>